<commit_message>
single eye-track entropy success
</commit_message>
<xml_diff>
--- a/tables/tables.xlsx
+++ b/tables/tables.xlsx
@@ -5,15 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\美学计算\eyeTrackingExp\text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\美学计算\eyeTrackingExp\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="5-1_score_category_sorted" sheetId="1" r:id="rId1"/>
     <sheet name="5-2_注视举例" sheetId="2" r:id="rId2"/>
+    <sheet name="6-1,weightless30values" sheetId="3" r:id="rId3"/>
+    <sheet name="6-2，weighless30anova" sheetId="4" r:id="rId4"/>
+    <sheet name="6-3，fix总数values" sheetId="5" r:id="rId5"/>
+    <sheet name="6-4，fix总数" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>得分排序</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,6 +56,65 @@
   </si>
   <si>
     <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Prob&gt;F</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>r = 0.5489</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p = 77.5%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去权热图30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fix总数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -272,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -311,6 +374,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1004,7 +1073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
@@ -1144,4 +1213,1127 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>18.725325393083999</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>18.693662991558298</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>19.098659119878899</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>18.182233603891</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>18.7854002840816</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>18.8642789697025</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>18.724921754368701</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>18.4115322593507</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>18.273414876029801</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>18.6407991480751</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>18.516287739974899</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>3.3333333E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>18.533404796003499</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>3.3333333E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>18.806881781889398</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>3.3333333E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>18.170972210924699</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>6.4516129032258104E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>18.520489911102999</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>6.4516129032258104E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>18.286165591586499</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>6.6666666999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>18.4214882577735</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>9.6774193548387094E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>18.620666382617902</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>18.158332647491498</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0.12903225806451599</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>18.467048387397</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0.19354838709677399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>18.024570227283601</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0.61290322580645196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>18.006691301712198</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.64516129032258096</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>18.106318574728601</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.67741935483870996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>18.603611403919199</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>18.367056900173999</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.70967741935483897</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>18.120741357090601</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0.76666666699999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>18.142130976581399</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.80645161290322598</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>18.5845871544098</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0.83870967741935498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>18.2708725121973</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.86666666699999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>18.3445152298507</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0.87096774193548399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>18.243035587932098</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.93548387096774199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>17.583824737030799</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0.93548387096774199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>18.305827646794299</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0.93548387096774199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>18.294174192666301</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.96666666700000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>18.040239034773901</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0.96666666700000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>18.113347729226899</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0.967741935483871</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>18.1499002072945</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0.967741935483871</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>18.551427995002499</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>18.485320159660699</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>18.1987027897767</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1.01285</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1.01285</v>
+      </c>
+      <c r="E2" s="13">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F2" s="13">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="13">
+        <v>2.3180200000000002</v>
+      </c>
+      <c r="C3" s="13">
+        <v>38</v>
+      </c>
+      <c r="D3" s="13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3.33087</v>
+      </c>
+      <c r="C4" s="13">
+        <v>39</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>302</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>301</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>309</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>289</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>310</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>307</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>298</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>292</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>295</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>294</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>318</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>3.3333333E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>303</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>3.3333333E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>322</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>3.3333333E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>289</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>6.4516129032258104E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>286</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>6.4516129032258104E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>299</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>6.6666666999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>290</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>9.6774193548387094E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>308</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>300</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0.12903225806451599</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>304</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0.19354838709677399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>321</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0.61290322580645196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>300</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.64516129032258096</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>292</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.67741935483870996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>294</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>301</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.70967741935483897</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>315</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0.76666666699999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>340</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.80645161290322598</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>317</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0.83870967741935498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>290</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.86666666699999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>303</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0.87096774193548399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>298</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.93548387096774199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>305</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0.93548387096774199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>316</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0.93548387096774199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>299</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.96666666700000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>301</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0.96666666700000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>298</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0.967741935483871</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>325</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0.967741935483871</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>324</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>314</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>316</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="14">
+        <v>585.23</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>585.22500000000002</v>
+      </c>
+      <c r="E2" s="14">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="F2" s="14">
+        <v>4.2900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="14">
+        <v>5068.1499999999996</v>
+      </c>
+      <c r="C3" s="14">
+        <v>38</v>
+      </c>
+      <c r="D3" s="14">
+        <v>133.37200000000001</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="14">
+        <v>5653.38</v>
+      </c>
+      <c r="C4" s="14">
+        <v>39</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>